<commit_message>
continue study kernels1.py datamissing processing
</commit_message>
<xml_diff>
--- a/venv/input_data/characteristics.xlsx
+++ b/venv/input_data/characteristics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -270,6 +270,14 @@
   </si>
   <si>
     <t>微小的线性相关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泳池质量，删除/重建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺失值太多删除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -622,7 +630,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -895,7 +903,9 @@
       <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1180,7 +1190,9 @@
       <c r="D27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>

</xml_diff>